<commit_message>
synced crossbar with mcu pinout on schematic
</commit_message>
<xml_diff>
--- a/dwg/crossbar.xlsx
+++ b/dwg/crossbar.xlsx
@@ -449,9 +449,6 @@
     <t>TIM9_CH1</t>
   </si>
   <si>
-    <t>LED_USART</t>
-  </si>
-  <si>
     <t>FAN</t>
   </si>
   <si>
@@ -780,6 +777,9 @@
   </si>
   <si>
     <t>USART4_TX</t>
+  </si>
+  <si>
+    <t>LED_UART</t>
   </si>
 </sst>
 </file>
@@ -1150,9 +1150,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q7" sqref="Q7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1185,7 @@
         <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>29</v>
@@ -1200,10 +1200,10 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>48</v>
@@ -1212,7 +1212,7 @@
         <v>129</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>17</v>
@@ -1229,7 +1229,7 @@
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -1253,7 +1253,7 @@
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -1277,7 +1277,7 @@
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q5">
         <v>4</v>
@@ -1309,7 +1309,7 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -1333,7 +1333,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1359,7 +1359,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Q8">
         <v>7</v>
@@ -1398,7 +1398,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1409,14 +1409,14 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Q10" s="2">
         <v>9</v>
@@ -1431,7 +1431,7 @@
         <v>120</v>
       </c>
       <c r="K11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="Q11">
         <v>10</v>
@@ -1445,7 +1445,7 @@
         <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E12" t="s">
         <v>57</v>
@@ -1454,10 +1454,10 @@
         <v>57</v>
       </c>
       <c r="H12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Q12">
         <v>11</v>
@@ -1476,7 +1476,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1484,7 +1484,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" s="2" t="s">
@@ -1500,26 +1500,26 @@
         <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H14" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>220</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>221</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -1537,7 +1537,7 @@
         <v>67</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>141</v>
+        <v>251</v>
       </c>
       <c r="E15" t="s">
         <v>68</v>
@@ -1602,10 +1602,10 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -1629,11 +1629,11 @@
         <v>26</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M18" s="4"/>
       <c r="O18" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P18" t="s">
         <v>40</v>
@@ -1660,13 +1660,13 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P19" s="2" t="s">
         <v>123</v>
@@ -1681,7 +1681,7 @@
         <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Q20">
         <v>19</v>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>126</v>
@@ -1735,7 +1735,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -1743,7 +1743,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
@@ -1763,7 +1763,7 @@
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
@@ -1787,7 +1787,7 @@
         <v>37</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -1813,7 +1813,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -1867,9 +1867,6 @@
       <c r="B28" t="s">
         <v>50</v>
       </c>
-      <c r="E28" t="s">
-        <v>27</v>
-      </c>
       <c r="G28" t="s">
         <v>27</v>
       </c>
@@ -1882,7 +1879,7 @@
         <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Q29">
         <v>28</v>
@@ -1895,12 +1892,6 @@
       <c r="B30" t="s">
         <v>31</v>
       </c>
-      <c r="D30" t="s">
-        <v>106</v>
-      </c>
-      <c r="E30" t="s">
-        <v>32</v>
-      </c>
       <c r="G30" t="s">
         <v>32</v>
       </c>
@@ -1913,7 +1904,7 @@
         <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Q31">
         <v>30</v>
@@ -1926,12 +1917,6 @@
       <c r="B32" t="s">
         <v>36</v>
       </c>
-      <c r="D32" t="s">
-        <v>105</v>
-      </c>
-      <c r="E32" t="s">
-        <v>35</v>
-      </c>
       <c r="G32" t="s">
         <v>35</v>
       </c>
@@ -1945,12 +1930,6 @@
       </c>
       <c r="B33" t="s">
         <v>39</v>
-      </c>
-      <c r="D33" t="s">
-        <v>107</v>
-      </c>
-      <c r="E33" t="s">
-        <v>38</v>
       </c>
       <c r="G33" t="s">
         <v>38</v>
@@ -1991,11 +1970,11 @@
         <v>1</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L35" s="2"/>
       <c r="M35" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -2014,11 +1993,8 @@
       <c r="B36" t="s">
         <v>13</v>
       </c>
-      <c r="E36" t="s">
-        <v>51</v>
-      </c>
       <c r="G36" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J36" t="s">
         <v>16</v>
@@ -2040,16 +2016,14 @@
       </c>
       <c r="C37"/>
       <c r="D37"/>
-      <c r="E37" t="s">
-        <v>51</v>
-      </c>
+      <c r="E37"/>
       <c r="F37"/>
       <c r="G37"/>
       <c r="H37"/>
       <c r="I37"/>
       <c r="J37"/>
       <c r="K37" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L37"/>
       <c r="M37"/>
@@ -2070,7 +2044,7 @@
       </c>
       <c r="C38"/>
       <c r="D38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E38" t="s">
         <v>51</v>
@@ -2081,7 +2055,7 @@
       <c r="I38"/>
       <c r="J38"/>
       <c r="K38" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L38"/>
       <c r="M38"/>
@@ -2098,13 +2072,13 @@
         <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O39" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q39">
         <v>38</v>
@@ -2119,7 +2093,7 @@
         <v>30</v>
       </c>
       <c r="D40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E40" t="s">
         <v>51</v>
@@ -2133,7 +2107,7 @@
         <v>55</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C41" s="4"/>
       <c r="E41" s="4"/>
@@ -2145,7 +2119,7 @@
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
@@ -2166,7 +2140,9 @@
       <c r="D42" t="s">
         <v>104</v>
       </c>
-      <c r="E42" s="4"/>
+      <c r="E42" t="s">
+        <v>51</v>
+      </c>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
@@ -2190,7 +2166,7 @@
         <v>57</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C43" s="4"/>
       <c r="E43" s="4"/>
@@ -2221,7 +2197,9 @@
       <c r="D44" t="s">
         <v>103</v>
       </c>
-      <c r="E44" s="4"/>
+      <c r="E44" t="s">
+        <v>51</v>
+      </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
@@ -2363,7 +2341,7 @@
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
@@ -2387,7 +2365,7 @@
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
@@ -2429,7 +2407,7 @@
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
       <c r="P51" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Q51" s="2" t="s">
         <v>134</v>
@@ -2443,7 +2421,7 @@
         <v>71</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -2459,7 +2437,7 @@
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
       <c r="P52" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="Q52" s="2" t="s">
         <v>134</v>
@@ -2473,7 +2451,7 @@
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
@@ -2497,7 +2475,7 @@
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
@@ -2521,7 +2499,7 @@
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
@@ -2545,7 +2523,7 @@
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
@@ -2569,7 +2547,7 @@
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
@@ -2593,7 +2571,7 @@
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
@@ -2617,7 +2595,7 @@
         <v>12</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -2633,7 +2611,7 @@
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
       <c r="P59" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Q59" s="2"/>
       <c r="R59" s="2">
@@ -2645,7 +2623,7 @@
         <v>13</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -2661,7 +2639,7 @@
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
       <c r="P60" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Q60" s="2"/>
       <c r="R60" s="2">
@@ -2701,7 +2679,7 @@
         <v>9</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -2717,7 +2695,7 @@
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
       <c r="P62" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="Q62" s="2"/>
       <c r="R62" s="2">
@@ -2732,7 +2710,7 @@
         <v>114</v>
       </c>
       <c r="I63" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="R63">
         <v>11</v>
@@ -2743,7 +2721,7 @@
         <v>7</v>
       </c>
       <c r="B64" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="R64">
         <v>12</v>
@@ -2765,7 +2743,7 @@
         <v>4</v>
       </c>
       <c r="B66" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I66" t="s">
         <v>140</v>
@@ -2796,7 +2774,7 @@
         <v>2</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -2812,7 +2790,7 @@
       <c r="N68" s="2"/>
       <c r="O68" s="2"/>
       <c r="P68" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Q68" s="2"/>
       <c r="R68" s="2">
@@ -2840,7 +2818,7 @@
       <c r="N69" s="2"/>
       <c r="O69" s="2"/>
       <c r="P69" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Q69" s="2"/>
       <c r="R69" s="2">
@@ -2852,7 +2830,7 @@
         <v>98</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -2868,7 +2846,7 @@
       <c r="N70" s="2"/>
       <c r="O70" s="2"/>
       <c r="P70" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Q70" s="2"/>
       <c r="R70" s="2">
@@ -2892,13 +2870,13 @@
         <v>93</v>
       </c>
       <c r="I71" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J71" t="s">
         <v>7</v>
       </c>
       <c r="L71" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="R71">
         <v>19</v>
@@ -2920,13 +2898,13 @@
         <v>95</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J72" s="2" t="s">
         <v>15</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L72" s="2"/>
       <c r="M72" s="2"/>
@@ -2945,7 +2923,7 @@
         <v>94</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
@@ -2968,7 +2946,7 @@
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="R74" s="4">
         <v>22</v>
@@ -2995,7 +2973,7 @@
       </c>
       <c r="K75" s="2"/>
       <c r="L75" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M75" s="2" t="s">
         <v>49</v>
@@ -3031,10 +3009,10 @@
       </c>
       <c r="K76" s="4"/>
       <c r="L76" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M76" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="R76">
         <v>24</v>
@@ -3048,13 +3026,13 @@
         <v>62</v>
       </c>
       <c r="F77" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H77" t="s">
         <v>61</v>
       </c>
       <c r="K77" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="R77">
         <v>25</v>
@@ -3065,7 +3043,7 @@
         <v>91</v>
       </c>
       <c r="B78" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C78"/>
       <c r="D78"/>
@@ -3078,7 +3056,7 @@
       <c r="I78"/>
       <c r="J78"/>
       <c r="K78" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L78"/>
       <c r="M78"/>
@@ -3095,7 +3073,7 @@
         <v>88</v>
       </c>
       <c r="B79" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C79"/>
       <c r="D79"/>
@@ -3121,16 +3099,16 @@
         <v>89</v>
       </c>
       <c r="B80" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F80" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G80" t="s">
         <v>57</v>
       </c>
       <c r="K80" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R80">
         <v>28</v>
@@ -3171,7 +3149,7 @@
         <v>87</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C82" s="4"/>
       <c r="D82"/>
@@ -3184,7 +3162,7 @@
       <c r="K82" s="4"/>
       <c r="L82" s="4"/>
       <c r="M82" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N82" s="4"/>
       <c r="O82" s="4"/>
@@ -3199,7 +3177,7 @@
         <v>84</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C83" s="4"/>
       <c r="E83" s="4"/>
@@ -3224,7 +3202,7 @@
         <v>85</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
@@ -3240,7 +3218,7 @@
       <c r="N84" s="2"/>
       <c r="O84" s="2"/>
       <c r="P84" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q84" s="2"/>
       <c r="R84" s="2">
@@ -3252,7 +3230,7 @@
         <v>82</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C85" s="4"/>
       <c r="E85" s="4"/>
@@ -3277,11 +3255,11 @@
         <v>83</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C86" s="4"/>
       <c r="D86" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E86" s="4" t="s">
         <v>51</v>
@@ -3295,7 +3273,7 @@
       <c r="L86" s="4"/>
       <c r="M86" s="4"/>
       <c r="N86" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O86" s="4"/>
       <c r="P86" s="4"/>
@@ -3309,7 +3287,7 @@
         <v>80</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
@@ -3321,13 +3299,13 @@
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
       <c r="L87" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
       <c r="O87" s="2"/>
       <c r="P87" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Q87" s="2"/>
       <c r="R87" s="2">
@@ -3339,13 +3317,15 @@
         <v>81</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C88" s="4"/>
       <c r="D88" t="s">
-        <v>150</v>
-      </c>
-      <c r="E88" s="4"/>
+        <v>149</v>
+      </c>
+      <c r="E88" t="s">
+        <v>51</v>
+      </c>
       <c r="F88" s="4"/>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
@@ -3367,7 +3347,7 @@
         <v>78</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
@@ -3379,17 +3359,17 @@
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
       <c r="L89" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M89" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N89" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O89" s="2"/>
       <c r="P89" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="Q89" s="2"/>
       <c r="R89" s="2">
@@ -3401,22 +3381,22 @@
         <v>80</v>
       </c>
       <c r="B90" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E90" t="s">
         <v>51</v>
       </c>
       <c r="L90" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M90" t="s">
         <v>111</v>
       </c>
       <c r="N90" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R90">
         <v>38</v>
@@ -3427,13 +3407,13 @@
         <v>76</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
@@ -3445,7 +3425,7 @@
       <c r="N91" s="2"/>
       <c r="O91" s="2"/>
       <c r="P91" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q91" s="2"/>
       <c r="R91" s="2">
@@ -3457,13 +3437,13 @@
         <v>77</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
       <c r="F92" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G92" s="5" t="s">
         <v>55</v>
@@ -3472,10 +3452,10 @@
       <c r="I92" s="5"/>
       <c r="J92" s="5"/>
       <c r="K92" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L92" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M92" s="5"/>
       <c r="N92" s="5"/>
@@ -3506,7 +3486,7 @@
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
       <c r="M93" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N93" s="2"/>
       <c r="O93" s="2"/>
@@ -3523,13 +3503,13 @@
         <v>72</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
       <c r="F94" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
@@ -3541,7 +3521,7 @@
       <c r="N94" s="2"/>
       <c r="O94" s="2"/>
       <c r="P94" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q94" s="2"/>
       <c r="R94" s="2">
@@ -3556,7 +3536,10 @@
         <v>2</v>
       </c>
       <c r="D95" t="s">
-        <v>148</v>
+        <v>147</v>
+      </c>
+      <c r="E95" t="s">
+        <v>27</v>
       </c>
       <c r="G95" t="s">
         <v>27</v>
@@ -3607,13 +3590,13 @@
         <v>65</v>
       </c>
       <c r="B97" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H97" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I97" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="R97">
         <v>45</v>
@@ -3630,13 +3613,13 @@
         <v>51</v>
       </c>
       <c r="F98" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H98" t="s">
         <v>126</v>
       </c>
       <c r="I98" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J98" t="s">
         <v>14</v>
@@ -3659,7 +3642,7 @@
         <v>128</v>
       </c>
       <c r="N99" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="P99" t="s">
         <v>130</v>
@@ -3673,7 +3656,7 @@
         <v>64</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
@@ -3684,18 +3667,18 @@
         <v>26</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
       <c r="M100" s="2"/>
       <c r="N100" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O100" s="2"/>
       <c r="P100" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q100" s="2"/>
       <c r="R100" s="2">
@@ -3707,7 +3690,7 @@
       <c r="B101" s="6"/>
       <c r="C101" s="6"/>
       <c r="D101" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E101" s="6"/>
       <c r="F101" s="6"/>
@@ -3731,7 +3714,7 @@
       <c r="B102" s="6"/>
       <c r="C102" s="6"/>
       <c r="D102" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E102" s="6"/>
       <c r="F102" s="6"/>
@@ -3750,15 +3733,36 @@
         <v>50</v>
       </c>
     </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D104" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D105" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D106" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D107" t="s">
+      <c r="D107" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="E107" t="s">
+      <c r="E107" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="H107" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -3776,7 +3780,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3851,7 +3855,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Initial part placement on layout complete
</commit_message>
<xml_diff>
--- a/dwg/crossbar.xlsx
+++ b/dwg/crossbar.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="252">
   <si>
     <t>PB10</t>
   </si>
@@ -161,9 +161,6 @@
     <t>TIM1</t>
   </si>
   <si>
-    <t>TIM2</t>
-  </si>
-  <si>
     <t>I2C1</t>
   </si>
   <si>
@@ -780,6 +777,9 @@
   </si>
   <si>
     <t>LED_UART</t>
+  </si>
+  <si>
+    <t>TIM8</t>
   </si>
 </sst>
 </file>
@@ -1151,8 +1151,8 @@
   <dimension ref="A1:R107"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1185,7 @@
         <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>29</v>
@@ -1194,25 +1194,25 @@
         <v>25</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>226</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>17</v>
@@ -1229,7 +1229,7 @@
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -1253,7 +1253,7 @@
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -1277,7 +1277,7 @@
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Q5">
         <v>4</v>
@@ -1309,7 +1309,7 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -1333,7 +1333,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1359,7 +1359,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Q8">
         <v>7</v>
@@ -1370,7 +1370,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1386,7 +1386,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q9" s="2">
         <v>8</v>
@@ -1398,7 +1398,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1409,14 +1409,14 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Q10" s="2">
         <v>9</v>
@@ -1428,10 +1428,10 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="Q11">
         <v>10</v>
@@ -1442,22 +1442,16 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" t="s">
         <v>56</v>
       </c>
-      <c r="D12" t="s">
-        <v>141</v>
-      </c>
-      <c r="E12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" t="s">
-        <v>57</v>
-      </c>
       <c r="H12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q12">
         <v>11</v>
@@ -1468,7 +1462,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1476,7 +1470,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1484,11 +1478,11 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q13" s="2">
         <v>12</v>
@@ -1500,26 +1494,26 @@
         <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H14" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>219</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>220</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -1534,25 +1528,25 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="E15" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="E15" t="s">
-        <v>68</v>
-      </c>
       <c r="G15" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="H15" t="s">
         <v>137</v>
       </c>
-      <c r="H15" t="s">
-        <v>138</v>
-      </c>
       <c r="I15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q15">
         <v>14</v>
@@ -1568,7 +1562,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1579,7 +1573,7 @@
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q16" s="2">
         <v>15</v>
@@ -1591,7 +1585,7 @@
         <v>29</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1602,16 +1596,16 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q17" s="2">
         <v>16</v>
@@ -1629,11 +1623,11 @@
         <v>26</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="M18" s="4"/>
       <c r="O18" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P18" t="s">
         <v>40</v>
@@ -1647,7 +1641,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1655,21 +1649,21 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Q19" s="2">
         <v>18</v>
@@ -1681,7 +1675,7 @@
         <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q20">
         <v>19</v>
@@ -1692,7 +1686,7 @@
         <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q21">
         <v>20</v>
@@ -1706,16 +1700,10 @@
         <v>12</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>126</v>
-      </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -1735,7 +1723,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -1743,7 +1731,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
@@ -1763,7 +1751,7 @@
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
@@ -1787,7 +1775,7 @@
         <v>37</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -1813,7 +1801,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -1865,7 +1853,7 @@
         <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G28" t="s">
         <v>27</v>
@@ -1879,7 +1867,7 @@
         <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q29">
         <v>28</v>
@@ -1904,7 +1892,7 @@
         <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Q31">
         <v>30</v>
@@ -1943,7 +1931,7 @@
         <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D34" s="4"/>
       <c r="Q34">
@@ -1962,7 +1950,7 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
@@ -1970,16 +1958,16 @@
         <v>1</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L35" s="2"/>
       <c r="M35" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
       <c r="P35" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q35" s="2">
         <v>34</v>
@@ -1994,14 +1982,14 @@
         <v>13</v>
       </c>
       <c r="G36" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J36" t="s">
         <v>16</v>
       </c>
       <c r="K36" s="4"/>
       <c r="M36" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q36">
         <v>35</v>
@@ -2012,7 +2000,7 @@
         <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C37"/>
       <c r="D37"/>
@@ -2023,7 +2011,7 @@
       <c r="I37"/>
       <c r="J37"/>
       <c r="K37" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L37"/>
       <c r="M37"/>
@@ -2043,19 +2031,13 @@
         <v>28</v>
       </c>
       <c r="C38"/>
-      <c r="D38" t="s">
-        <v>145</v>
-      </c>
-      <c r="E38" t="s">
-        <v>51</v>
-      </c>
       <c r="F38"/>
       <c r="G38"/>
       <c r="H38"/>
       <c r="I38"/>
       <c r="J38"/>
       <c r="K38" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L38"/>
       <c r="M38"/>
@@ -2072,13 +2054,13 @@
         <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="O39" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q39">
         <v>38</v>
@@ -2092,12 +2074,6 @@
       <c r="B40" t="s">
         <v>30</v>
       </c>
-      <c r="D40" t="s">
-        <v>146</v>
-      </c>
-      <c r="E40" t="s">
-        <v>51</v>
-      </c>
       <c r="Q40">
         <v>39</v>
       </c>
@@ -2107,7 +2083,7 @@
         <v>55</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C41" s="4"/>
       <c r="E41" s="4"/>
@@ -2119,7 +2095,7 @@
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
@@ -2134,15 +2110,9 @@
         <v>56</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C42" s="4"/>
-      <c r="D42" t="s">
-        <v>104</v>
-      </c>
-      <c r="E42" t="s">
-        <v>51</v>
-      </c>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
@@ -2151,7 +2121,7 @@
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
@@ -2166,10 +2136,9 @@
         <v>57</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C43" s="4"/>
-      <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
@@ -2191,15 +2160,9 @@
         <v>58</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C44" s="4"/>
-      <c r="D44" t="s">
-        <v>103</v>
-      </c>
-      <c r="E44" t="s">
-        <v>51</v>
-      </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
@@ -2221,7 +2184,7 @@
         <v>59</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -2229,7 +2192,7 @@
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -2239,7 +2202,7 @@
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
       <c r="P45" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q45" s="2">
         <v>44</v>
@@ -2251,7 +2214,7 @@
         <v>60</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -2259,7 +2222,7 @@
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
@@ -2269,7 +2232,7 @@
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
       <c r="P46" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q46" s="2">
         <v>45</v>
@@ -2281,7 +2244,7 @@
         <v>61</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -2289,7 +2252,7 @@
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -2299,7 +2262,7 @@
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
       <c r="P47" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q47" s="2">
         <v>46</v>
@@ -2311,7 +2274,7 @@
         <v>62</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -2319,7 +2282,7 @@
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
@@ -2329,7 +2292,7 @@
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
       <c r="P48" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q48" s="2">
         <v>47</v>
@@ -2341,7 +2304,7 @@
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
@@ -2365,7 +2328,7 @@
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
@@ -2407,13 +2370,13 @@
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
       <c r="P51" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q51" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R51" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
@@ -2421,7 +2384,7 @@
         <v>71</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -2437,13 +2400,13 @@
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
       <c r="P52" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Q52" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R52" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
@@ -2451,7 +2414,7 @@
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
@@ -2475,7 +2438,7 @@
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
@@ -2499,7 +2462,7 @@
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
@@ -2523,7 +2486,7 @@
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
@@ -2547,7 +2510,7 @@
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
@@ -2571,7 +2534,7 @@
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
@@ -2595,7 +2558,7 @@
         <v>12</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -2611,7 +2574,7 @@
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
       <c r="P59" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Q59" s="2"/>
       <c r="R59" s="2">
@@ -2623,7 +2586,7 @@
         <v>13</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -2639,7 +2602,7 @@
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
       <c r="P60" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Q60" s="2"/>
       <c r="R60" s="2">
@@ -2651,7 +2614,7 @@
         <v>8</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -2667,7 +2630,7 @@
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
       <c r="P61" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q61" s="2"/>
       <c r="R61" s="2">
@@ -2679,7 +2642,7 @@
         <v>9</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -2695,7 +2658,7 @@
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
       <c r="P62" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="Q62" s="2"/>
       <c r="R62" s="2">
@@ -2707,10 +2670,16 @@
         <v>5</v>
       </c>
       <c r="B63" t="s">
-        <v>114</v>
+        <v>113</v>
+      </c>
+      <c r="D63" t="s">
+        <v>144</v>
+      </c>
+      <c r="E63" t="s">
+        <v>50</v>
       </c>
       <c r="I63" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="R63">
         <v>11</v>
@@ -2721,7 +2690,13 @@
         <v>7</v>
       </c>
       <c r="B64" t="s">
-        <v>188</v>
+        <v>187</v>
+      </c>
+      <c r="D64" t="s">
+        <v>103</v>
+      </c>
+      <c r="E64" t="s">
+        <v>50</v>
       </c>
       <c r="R64">
         <v>12</v>
@@ -2732,7 +2707,13 @@
         <v>3</v>
       </c>
       <c r="B65" t="s">
-        <v>115</v>
+        <v>114</v>
+      </c>
+      <c r="D65" t="s">
+        <v>145</v>
+      </c>
+      <c r="E65" t="s">
+        <v>50</v>
       </c>
       <c r="R65">
         <v>13</v>
@@ -2743,10 +2724,16 @@
         <v>4</v>
       </c>
       <c r="B66" t="s">
-        <v>204</v>
+        <v>203</v>
+      </c>
+      <c r="D66" t="s">
+        <v>102</v>
+      </c>
+      <c r="E66" t="s">
+        <v>50</v>
       </c>
       <c r="I66" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="R66">
         <v>14</v>
@@ -2757,13 +2744,13 @@
         <v>1</v>
       </c>
       <c r="B67" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D67" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E67" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R67">
         <v>15</v>
@@ -2774,7 +2761,7 @@
         <v>2</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -2790,7 +2777,7 @@
       <c r="N68" s="2"/>
       <c r="O68" s="2"/>
       <c r="P68" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Q68" s="2"/>
       <c r="R68" s="2">
@@ -2802,7 +2789,7 @@
         <v>97</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -2818,7 +2805,7 @@
       <c r="N69" s="2"/>
       <c r="O69" s="2"/>
       <c r="P69" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Q69" s="2"/>
       <c r="R69" s="2">
@@ -2830,7 +2817,7 @@
         <v>98</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -2846,7 +2833,7 @@
       <c r="N70" s="2"/>
       <c r="O70" s="2"/>
       <c r="P70" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Q70" s="2"/>
       <c r="R70" s="2">
@@ -2861,22 +2848,22 @@
         <v>8</v>
       </c>
       <c r="D71" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E71" t="s">
         <v>7</v>
       </c>
       <c r="H71" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I71" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J71" t="s">
         <v>7</v>
       </c>
       <c r="L71" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="R71">
         <v>19</v>
@@ -2887,7 +2874,7 @@
         <v>96</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
@@ -2895,23 +2882,23 @@
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J72" s="2" t="s">
         <v>15</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L72" s="2"/>
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
       <c r="O72" s="2"/>
       <c r="P72" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Q72" s="2"/>
       <c r="R72" s="2">
@@ -2923,7 +2910,7 @@
         <v>94</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
@@ -2946,7 +2933,7 @@
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="R74" s="4">
         <v>22</v>
@@ -2965,7 +2952,7 @@
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I75" s="2"/>
       <c r="J75" s="2" t="s">
@@ -2973,10 +2960,10 @@
       </c>
       <c r="K75" s="2"/>
       <c r="L75" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="M75" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N75" s="2"/>
       <c r="O75" s="2"/>
@@ -2996,23 +2983,23 @@
         <v>11</v>
       </c>
       <c r="D76" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E76" t="s">
         <v>15</v>
       </c>
       <c r="H76" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J76" t="s">
         <v>15</v>
       </c>
       <c r="K76" s="4"/>
       <c r="L76" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M76" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="R76">
         <v>24</v>
@@ -3023,16 +3010,16 @@
         <v>90</v>
       </c>
       <c r="B77" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F77" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H77" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K77" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R77">
         <v>25</v>
@@ -3043,7 +3030,7 @@
         <v>91</v>
       </c>
       <c r="B78" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C78"/>
       <c r="D78"/>
@@ -3056,7 +3043,7 @@
       <c r="I78"/>
       <c r="J78"/>
       <c r="K78" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L78"/>
       <c r="M78"/>
@@ -3073,7 +3060,7 @@
         <v>88</v>
       </c>
       <c r="B79" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C79"/>
       <c r="D79"/>
@@ -3099,16 +3086,16 @@
         <v>89</v>
       </c>
       <c r="B80" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F80" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G80" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K80" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="R80">
         <v>28</v>
@@ -3119,7 +3106,7 @@
         <v>86</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
@@ -3132,12 +3119,12 @@
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
       <c r="M81" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N81" s="2"/>
       <c r="O81" s="2"/>
       <c r="P81" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Q81" s="2"/>
       <c r="R81" s="2">
@@ -3149,11 +3136,9 @@
         <v>87</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C82" s="4"/>
-      <c r="D82"/>
-      <c r="E82" s="4"/>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
@@ -3162,7 +3147,7 @@
       <c r="K82" s="4"/>
       <c r="L82" s="4"/>
       <c r="M82" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N82" s="4"/>
       <c r="O82" s="4"/>
@@ -3177,7 +3162,7 @@
         <v>84</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C83" s="4"/>
       <c r="E83" s="4"/>
@@ -3202,7 +3187,7 @@
         <v>85</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
@@ -3218,7 +3203,7 @@
       <c r="N84" s="2"/>
       <c r="O84" s="2"/>
       <c r="P84" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="Q84" s="2"/>
       <c r="R84" s="2">
@@ -3230,7 +3215,7 @@
         <v>82</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C85" s="4"/>
       <c r="E85" s="4"/>
@@ -3255,14 +3240,14 @@
         <v>83</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C86" s="4"/>
       <c r="D86" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F86" s="4"/>
       <c r="G86" s="4"/>
@@ -3273,7 +3258,7 @@
       <c r="L86" s="4"/>
       <c r="M86" s="4"/>
       <c r="N86" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O86" s="4"/>
       <c r="P86" s="4"/>
@@ -3287,7 +3272,7 @@
         <v>80</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
@@ -3299,13 +3284,13 @@
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
       <c r="L87" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
       <c r="O87" s="2"/>
       <c r="P87" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="Q87" s="2"/>
       <c r="R87" s="2">
@@ -3317,14 +3302,14 @@
         <v>81</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C88" s="4"/>
       <c r="D88" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E88" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F88" s="4"/>
       <c r="G88" s="4"/>
@@ -3347,7 +3332,7 @@
         <v>78</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
@@ -3359,17 +3344,17 @@
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
       <c r="L89" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="M89" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N89" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O89" s="2"/>
       <c r="P89" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Q89" s="2"/>
       <c r="R89" s="2">
@@ -3381,22 +3366,22 @@
         <v>80</v>
       </c>
       <c r="B90" t="s">
+        <v>151</v>
+      </c>
+      <c r="D90" t="s">
+        <v>158</v>
+      </c>
+      <c r="E90" t="s">
+        <v>50</v>
+      </c>
+      <c r="L90" t="s">
+        <v>243</v>
+      </c>
+      <c r="M90" t="s">
+        <v>110</v>
+      </c>
+      <c r="N90" t="s">
         <v>152</v>
-      </c>
-      <c r="D90" t="s">
-        <v>159</v>
-      </c>
-      <c r="E90" t="s">
-        <v>51</v>
-      </c>
-      <c r="L90" t="s">
-        <v>244</v>
-      </c>
-      <c r="M90" t="s">
-        <v>111</v>
-      </c>
-      <c r="N90" t="s">
-        <v>153</v>
       </c>
       <c r="R90">
         <v>38</v>
@@ -3407,13 +3392,13 @@
         <v>76</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
@@ -3425,7 +3410,7 @@
       <c r="N91" s="2"/>
       <c r="O91" s="2"/>
       <c r="P91" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Q91" s="2"/>
       <c r="R91" s="2">
@@ -3437,25 +3422,25 @@
         <v>77</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
       <c r="F92" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H92" s="5"/>
       <c r="I92" s="5"/>
       <c r="J92" s="5"/>
       <c r="K92" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L92" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M92" s="5"/>
       <c r="N92" s="5"/>
@@ -3486,7 +3471,7 @@
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
       <c r="M93" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N93" s="2"/>
       <c r="O93" s="2"/>
@@ -3503,13 +3488,13 @@
         <v>72</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
       <c r="F94" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
@@ -3521,7 +3506,7 @@
       <c r="N94" s="2"/>
       <c r="O94" s="2"/>
       <c r="P94" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Q94" s="2"/>
       <c r="R94" s="2">
@@ -3536,7 +3521,7 @@
         <v>2</v>
       </c>
       <c r="D95" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E95" t="s">
         <v>27</v>
@@ -3573,7 +3558,7 @@
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
       <c r="M96" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N96" s="2"/>
       <c r="O96" s="2"/>
@@ -3590,13 +3575,13 @@
         <v>65</v>
       </c>
       <c r="B97" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H97" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I97" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="R97">
         <v>45</v>
@@ -3609,17 +3594,20 @@
       <c r="B98" t="s">
         <v>10</v>
       </c>
-      <c r="E98" t="s">
-        <v>51</v>
+      <c r="D98" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="F98" t="s">
+        <v>159</v>
+      </c>
+      <c r="H98" t="s">
+        <v>125</v>
+      </c>
+      <c r="I98" t="s">
         <v>160</v>
-      </c>
-      <c r="H98" t="s">
-        <v>126</v>
-      </c>
-      <c r="I98" t="s">
-        <v>161</v>
       </c>
       <c r="J98" t="s">
         <v>14</v>
@@ -3633,19 +3621,25 @@
         <v>63</v>
       </c>
       <c r="B99" t="s">
+        <v>126</v>
+      </c>
+      <c r="D99" t="s">
+        <v>140</v>
+      </c>
+      <c r="E99" t="s">
         <v>127</v>
       </c>
       <c r="H99" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I99" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P99" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="R99">
         <v>47</v>
@@ -3656,7 +3650,7 @@
         <v>64</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
@@ -3667,18 +3661,18 @@
         <v>26</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
       <c r="M100" s="2"/>
       <c r="N100" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="O100" s="2"/>
       <c r="P100" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q100" s="2"/>
       <c r="R100" s="2">
@@ -3690,7 +3684,7 @@
       <c r="B101" s="6"/>
       <c r="C101" s="6"/>
       <c r="D101" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E101" s="6"/>
       <c r="F101" s="6"/>
@@ -3714,7 +3708,7 @@
       <c r="B102" s="6"/>
       <c r="C102" s="6"/>
       <c r="D102" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E102" s="6"/>
       <c r="F102" s="6"/>
@@ -3735,7 +3729,7 @@
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D104" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E104" s="4" t="s">
         <v>32</v>
@@ -3743,7 +3737,7 @@
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D105" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E105" s="4" t="s">
         <v>35</v>
@@ -3751,7 +3745,7 @@
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D106" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E106" s="4" t="s">
         <v>38</v>
@@ -3759,11 +3753,9 @@
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D107" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E107" s="4" t="s">
-        <v>15</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="E107" s="4"/>
     </row>
   </sheetData>
   <sortState ref="A2:R102">
@@ -3780,7 +3772,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3807,7 +3799,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
         <v>58</v>
@@ -3818,20 +3810,20 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>251</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
@@ -3839,10 +3831,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -3867,77 +3859,77 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved all components inside the disc envelope
</commit_message>
<xml_diff>
--- a/dwg/crossbar.xlsx
+++ b/dwg/crossbar.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="250">
   <si>
     <t>PB10</t>
   </si>
@@ -330,12 +330,6 @@
   </si>
   <si>
     <t>Blue LED</t>
-  </si>
-  <si>
-    <t>Push Button Down</t>
-  </si>
-  <si>
-    <t>Push Button Up</t>
   </si>
   <si>
     <t>PB Down Int</t>
@@ -1151,8 +1145,8 @@
   <dimension ref="A1:R107"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I55" sqref="I55"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1179,7 @@
         <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>29</v>
@@ -1194,25 +1188,25 @@
         <v>25</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>47</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>17</v>
@@ -1229,7 +1223,7 @@
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -1253,7 +1247,7 @@
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -1277,7 +1271,7 @@
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -1298,7 +1292,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="Q5">
         <v>4</v>
@@ -1309,7 +1303,7 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -1333,7 +1327,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1359,7 +1353,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Q8">
         <v>7</v>
@@ -1370,7 +1364,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1386,7 +1380,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="Q9" s="2">
         <v>8</v>
@@ -1398,7 +1392,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1409,14 +1403,14 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="Q10" s="2">
         <v>9</v>
@@ -1428,10 +1422,10 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K11" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="Q11">
         <v>10</v>
@@ -1448,10 +1442,10 @@
         <v>56</v>
       </c>
       <c r="H12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="Q12">
         <v>11</v>
@@ -1470,7 +1464,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1478,7 +1472,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" s="2" t="s">
@@ -1494,26 +1488,26 @@
         <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>218</v>
-      </c>
       <c r="I14" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -1531,19 +1525,19 @@
         <v>66</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E15" t="s">
         <v>67</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H15" t="s">
+        <v>135</v>
+      </c>
+      <c r="I15" t="s">
         <v>137</v>
-      </c>
-      <c r="I15" t="s">
-        <v>139</v>
       </c>
       <c r="M15" t="s">
         <v>67</v>
@@ -1585,7 +1579,7 @@
         <v>29</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1596,16 +1590,16 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="Q17" s="2">
         <v>16</v>
@@ -1623,11 +1617,11 @@
         <v>26</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M18" s="4"/>
       <c r="O18" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="P18" t="s">
         <v>40</v>
@@ -1654,16 +1648,16 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="Q19" s="2">
         <v>18</v>
@@ -1675,7 +1669,7 @@
         <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="Q20">
         <v>19</v>
@@ -1686,7 +1680,7 @@
         <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="Q21">
         <v>20</v>
@@ -1703,7 +1697,7 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -1723,7 +1717,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -1731,7 +1725,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
@@ -1751,7 +1745,7 @@
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
@@ -1775,7 +1769,7 @@
         <v>37</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -1801,7 +1795,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -1867,7 +1861,7 @@
         <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="Q29">
         <v>28</v>
@@ -1892,7 +1886,7 @@
         <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="Q31">
         <v>30</v>
@@ -1950,7 +1944,7 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
@@ -1958,16 +1952,16 @@
         <v>1</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L35" s="2"/>
       <c r="M35" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
       <c r="P35" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="Q35" s="2">
         <v>34</v>
@@ -1982,14 +1976,14 @@
         <v>13</v>
       </c>
       <c r="G36" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J36" t="s">
         <v>16</v>
       </c>
       <c r="K36" s="4"/>
       <c r="M36" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="Q36">
         <v>35</v>
@@ -2011,7 +2005,7 @@
       <c r="I37"/>
       <c r="J37"/>
       <c r="K37" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="L37"/>
       <c r="M37"/>
@@ -2037,7 +2031,7 @@
       <c r="I38"/>
       <c r="J38"/>
       <c r="K38" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L38"/>
       <c r="M38"/>
@@ -2054,13 +2048,13 @@
         <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="O39" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="Q39">
         <v>38</v>
@@ -2083,7 +2077,7 @@
         <v>55</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C41" s="4"/>
       <c r="E41" s="4"/>
@@ -2095,7 +2089,7 @@
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
@@ -2110,7 +2104,7 @@
         <v>56</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C42" s="4"/>
       <c r="F42" s="4"/>
@@ -2121,7 +2115,7 @@
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
@@ -2136,7 +2130,7 @@
         <v>57</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C43" s="4"/>
       <c r="F43" s="4"/>
@@ -2160,7 +2154,7 @@
         <v>58</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C44" s="4"/>
       <c r="F44" s="4"/>
@@ -2304,7 +2298,7 @@
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
@@ -2328,7 +2322,7 @@
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
@@ -2370,13 +2364,13 @@
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
       <c r="P51" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q51" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="R51" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
@@ -2384,7 +2378,7 @@
         <v>71</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -2400,13 +2394,13 @@
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
       <c r="P52" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="Q52" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="R52" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
@@ -2414,7 +2408,7 @@
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
@@ -2438,7 +2432,7 @@
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
@@ -2462,7 +2456,7 @@
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
@@ -2486,7 +2480,7 @@
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
@@ -2510,7 +2504,7 @@
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
@@ -2534,7 +2528,7 @@
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
@@ -2558,7 +2552,7 @@
         <v>12</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -2574,7 +2568,7 @@
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
       <c r="P59" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="Q59" s="2"/>
       <c r="R59" s="2">
@@ -2586,7 +2580,7 @@
         <v>13</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -2602,7 +2596,7 @@
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
       <c r="P60" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="Q60" s="2"/>
       <c r="R60" s="2">
@@ -2614,7 +2608,7 @@
         <v>8</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -2630,7 +2624,7 @@
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
       <c r="P61" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="Q61" s="2"/>
       <c r="R61" s="2">
@@ -2642,7 +2636,7 @@
         <v>9</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -2658,7 +2652,7 @@
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
       <c r="P62" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="Q62" s="2"/>
       <c r="R62" s="2">
@@ -2670,16 +2664,16 @@
         <v>5</v>
       </c>
       <c r="B63" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D63" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E63" t="s">
         <v>50</v>
       </c>
       <c r="I63" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="R63">
         <v>11</v>
@@ -2690,13 +2684,7 @@
         <v>7</v>
       </c>
       <c r="B64" t="s">
-        <v>187</v>
-      </c>
-      <c r="D64" t="s">
-        <v>103</v>
-      </c>
-      <c r="E64" t="s">
-        <v>50</v>
+        <v>185</v>
       </c>
       <c r="R64">
         <v>12</v>
@@ -2707,10 +2695,10 @@
         <v>3</v>
       </c>
       <c r="B65" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D65" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E65" t="s">
         <v>50</v>
@@ -2724,16 +2712,10 @@
         <v>4</v>
       </c>
       <c r="B66" t="s">
-        <v>203</v>
-      </c>
-      <c r="D66" t="s">
-        <v>102</v>
-      </c>
-      <c r="E66" t="s">
-        <v>50</v>
+        <v>201</v>
       </c>
       <c r="I66" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="R66">
         <v>14</v>
@@ -2744,10 +2726,10 @@
         <v>1</v>
       </c>
       <c r="B67" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D67" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E67" t="s">
         <v>50</v>
@@ -2761,7 +2743,7 @@
         <v>2</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -2777,7 +2759,7 @@
       <c r="N68" s="2"/>
       <c r="O68" s="2"/>
       <c r="P68" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="Q68" s="2"/>
       <c r="R68" s="2">
@@ -2789,7 +2771,7 @@
         <v>97</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -2805,7 +2787,7 @@
       <c r="N69" s="2"/>
       <c r="O69" s="2"/>
       <c r="P69" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="Q69" s="2"/>
       <c r="R69" s="2">
@@ -2817,7 +2799,7 @@
         <v>98</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -2833,7 +2815,7 @@
       <c r="N70" s="2"/>
       <c r="O70" s="2"/>
       <c r="P70" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="Q70" s="2"/>
       <c r="R70" s="2">
@@ -2848,7 +2830,7 @@
         <v>8</v>
       </c>
       <c r="D71" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E71" t="s">
         <v>7</v>
@@ -2857,13 +2839,13 @@
         <v>92</v>
       </c>
       <c r="I71" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="J71" t="s">
         <v>7</v>
       </c>
       <c r="L71" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="R71">
         <v>19</v>
@@ -2885,13 +2867,13 @@
         <v>94</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J72" s="2" t="s">
         <v>15</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="L72" s="2"/>
       <c r="M72" s="2"/>
@@ -2910,7 +2892,7 @@
         <v>94</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
@@ -2933,7 +2915,7 @@
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="R74" s="4">
         <v>22</v>
@@ -2960,7 +2942,7 @@
       </c>
       <c r="K75" s="2"/>
       <c r="L75" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="M75" s="2" t="s">
         <v>48</v>
@@ -2983,7 +2965,7 @@
         <v>11</v>
       </c>
       <c r="D76" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E76" t="s">
         <v>15</v>
@@ -2996,10 +2978,10 @@
       </c>
       <c r="K76" s="4"/>
       <c r="L76" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M76" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="R76">
         <v>24</v>
@@ -3013,13 +2995,13 @@
         <v>61</v>
       </c>
       <c r="F77" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H77" t="s">
         <v>60</v>
       </c>
       <c r="K77" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="R77">
         <v>25</v>
@@ -3030,7 +3012,7 @@
         <v>91</v>
       </c>
       <c r="B78" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C78"/>
       <c r="D78"/>
@@ -3043,7 +3025,7 @@
       <c r="I78"/>
       <c r="J78"/>
       <c r="K78" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L78"/>
       <c r="M78"/>
@@ -3060,7 +3042,7 @@
         <v>88</v>
       </c>
       <c r="B79" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C79"/>
       <c r="D79"/>
@@ -3086,16 +3068,16 @@
         <v>89</v>
       </c>
       <c r="B80" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F80" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G80" t="s">
         <v>56</v>
       </c>
       <c r="K80" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R80">
         <v>28</v>
@@ -3106,7 +3088,7 @@
         <v>86</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
@@ -3124,7 +3106,7 @@
       <c r="N81" s="2"/>
       <c r="O81" s="2"/>
       <c r="P81" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="Q81" s="2"/>
       <c r="R81" s="2">
@@ -3136,7 +3118,7 @@
         <v>87</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C82" s="4"/>
       <c r="F82" s="4"/>
@@ -3147,7 +3129,7 @@
       <c r="K82" s="4"/>
       <c r="L82" s="4"/>
       <c r="M82" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N82" s="4"/>
       <c r="O82" s="4"/>
@@ -3162,7 +3144,7 @@
         <v>84</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C83" s="4"/>
       <c r="E83" s="4"/>
@@ -3187,7 +3169,7 @@
         <v>85</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
@@ -3203,7 +3185,7 @@
       <c r="N84" s="2"/>
       <c r="O84" s="2"/>
       <c r="P84" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="Q84" s="2"/>
       <c r="R84" s="2">
@@ -3215,7 +3197,7 @@
         <v>82</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C85" s="4"/>
       <c r="E85" s="4"/>
@@ -3240,11 +3222,11 @@
         <v>83</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C86" s="4"/>
       <c r="D86" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E86" s="4" t="s">
         <v>50</v>
@@ -3258,7 +3240,7 @@
       <c r="L86" s="4"/>
       <c r="M86" s="4"/>
       <c r="N86" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="O86" s="4"/>
       <c r="P86" s="4"/>
@@ -3272,7 +3254,7 @@
         <v>80</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
@@ -3284,13 +3266,13 @@
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
       <c r="L87" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
       <c r="O87" s="2"/>
       <c r="P87" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="Q87" s="2"/>
       <c r="R87" s="2">
@@ -3302,11 +3284,11 @@
         <v>81</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C88" s="4"/>
       <c r="D88" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E88" t="s">
         <v>50</v>
@@ -3332,7 +3314,7 @@
         <v>78</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
@@ -3344,17 +3326,17 @@
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
       <c r="L89" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="M89" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="N89" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="O89" s="2"/>
       <c r="P89" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="Q89" s="2"/>
       <c r="R89" s="2">
@@ -3366,22 +3348,22 @@
         <v>80</v>
       </c>
       <c r="B90" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D90" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E90" t="s">
         <v>50</v>
       </c>
       <c r="L90" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M90" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="N90" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="R90">
         <v>38</v>
@@ -3392,13 +3374,13 @@
         <v>76</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
@@ -3410,7 +3392,7 @@
       <c r="N91" s="2"/>
       <c r="O91" s="2"/>
       <c r="P91" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="Q91" s="2"/>
       <c r="R91" s="2">
@@ -3422,13 +3404,13 @@
         <v>77</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
       <c r="F92" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G92" s="5" t="s">
         <v>54</v>
@@ -3437,10 +3419,10 @@
       <c r="I92" s="5"/>
       <c r="J92" s="5"/>
       <c r="K92" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="L92" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M92" s="5"/>
       <c r="N92" s="5"/>
@@ -3471,7 +3453,7 @@
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
       <c r="M93" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="N93" s="2"/>
       <c r="O93" s="2"/>
@@ -3488,13 +3470,13 @@
         <v>72</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
       <c r="F94" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
@@ -3506,7 +3488,7 @@
       <c r="N94" s="2"/>
       <c r="O94" s="2"/>
       <c r="P94" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="Q94" s="2"/>
       <c r="R94" s="2">
@@ -3521,7 +3503,7 @@
         <v>2</v>
       </c>
       <c r="D95" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E95" t="s">
         <v>27</v>
@@ -3575,13 +3557,13 @@
         <v>65</v>
       </c>
       <c r="B97" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H97" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I97" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="R97">
         <v>45</v>
@@ -3595,19 +3577,19 @@
         <v>10</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F98" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H98" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I98" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J98" t="s">
         <v>14</v>
@@ -3621,25 +3603,25 @@
         <v>63</v>
       </c>
       <c r="B99" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D99" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E99" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H99" t="s">
         <v>60</v>
       </c>
       <c r="I99" t="s">
+        <v>125</v>
+      </c>
+      <c r="N99" t="s">
+        <v>245</v>
+      </c>
+      <c r="P99" t="s">
         <v>127</v>
-      </c>
-      <c r="N99" t="s">
-        <v>247</v>
-      </c>
-      <c r="P99" t="s">
-        <v>129</v>
       </c>
       <c r="R99">
         <v>47</v>
@@ -3650,7 +3632,7 @@
         <v>64</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
@@ -3661,18 +3643,18 @@
         <v>26</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
       <c r="M100" s="2"/>
       <c r="N100" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O100" s="2"/>
       <c r="P100" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="Q100" s="2"/>
       <c r="R100" s="2">
@@ -3684,7 +3666,7 @@
       <c r="B101" s="6"/>
       <c r="C101" s="6"/>
       <c r="D101" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E101" s="6"/>
       <c r="F101" s="6"/>
@@ -3708,7 +3690,7 @@
       <c r="B102" s="6"/>
       <c r="C102" s="6"/>
       <c r="D102" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E102" s="6"/>
       <c r="F102" s="6"/>
@@ -3729,7 +3711,7 @@
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D104" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E104" s="4" t="s">
         <v>32</v>
@@ -3737,7 +3719,7 @@
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D105" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E105" s="4" t="s">
         <v>35</v>
@@ -3745,7 +3727,7 @@
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D106" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E106" s="4" t="s">
         <v>38</v>
@@ -3753,7 +3735,7 @@
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D107" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E107" s="4"/>
     </row>
@@ -3815,7 +3797,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B5" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
crossbar - updated positions of the leds
</commit_message>
<xml_diff>
--- a/dwg/crossbar.xlsx
+++ b/dwg/crossbar.xlsx
@@ -1169,8 +1169,8 @@
   <dimension ref="A1:R107"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,6 +1379,12 @@
       <c r="B8" t="s">
         <v>176</v>
       </c>
+      <c r="D8" t="s">
+        <v>250</v>
+      </c>
+      <c r="E8" t="s">
+        <v>50</v>
+      </c>
       <c r="Q8">
         <v>7</v>
       </c>
@@ -1448,12 +1454,6 @@
       <c r="B11" t="s">
         <v>117</v>
       </c>
-      <c r="D11" t="s">
-        <v>250</v>
-      </c>
-      <c r="E11" t="s">
-        <v>50</v>
-      </c>
       <c r="K11" t="s">
         <v>239</v>
       </c>
@@ -1467,6 +1467,12 @@
       </c>
       <c r="B12" t="s">
         <v>55</v>
+      </c>
+      <c r="D12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E12" t="s">
+        <v>50</v>
       </c>
       <c r="G12" t="s">
         <v>56</v>
@@ -1522,7 +1528,7 @@
       </c>
       <c r="C14" s="4"/>
       <c r="D14" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E14" t="s">
         <v>50</v>
@@ -1647,6 +1653,12 @@
       <c r="B18" t="s">
         <v>24</v>
       </c>
+      <c r="D18" t="s">
+        <v>253</v>
+      </c>
+      <c r="E18" t="s">
+        <v>50</v>
+      </c>
       <c r="H18" t="s">
         <v>26</v>
       </c>
@@ -1705,6 +1717,12 @@
       <c r="B20" t="s">
         <v>179</v>
       </c>
+      <c r="D20" t="s">
+        <v>254</v>
+      </c>
+      <c r="E20" t="s">
+        <v>50</v>
+      </c>
       <c r="Q20">
         <v>19</v>
       </c>
@@ -1716,12 +1734,6 @@
       <c r="B21" t="s">
         <v>121</v>
       </c>
-      <c r="D21" t="s">
-        <v>252</v>
-      </c>
-      <c r="E21" t="s">
-        <v>50</v>
-      </c>
       <c r="Q21">
         <v>20</v>
       </c>
@@ -1734,6 +1746,12 @@
         <v>12</v>
       </c>
       <c r="C22" s="4"/>
+      <c r="D22" t="s">
+        <v>255</v>
+      </c>
+      <c r="E22" t="s">
+        <v>50</v>
+      </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4" t="s">
@@ -1760,12 +1778,7 @@
         <v>139</v>
       </c>
       <c r="C23" s="4"/>
-      <c r="D23" t="s">
-        <v>253</v>
-      </c>
-      <c r="E23" t="s">
-        <v>50</v>
-      </c>
+      <c r="E23" s="6"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4" t="s">
@@ -1791,7 +1804,6 @@
       <c r="D24" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
@@ -1816,12 +1828,6 @@
         <v>173</v>
       </c>
       <c r="C25" s="4"/>
-      <c r="D25" t="s">
-        <v>254</v>
-      </c>
-      <c r="E25" t="s">
-        <v>50</v>
-      </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -1846,8 +1852,12 @@
         <v>202</v>
       </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
+      <c r="D26" t="s">
+        <v>256</v>
+      </c>
+      <c r="E26" t="s">
+        <v>50</v>
+      </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -1872,12 +1882,6 @@
         <v>30</v>
       </c>
       <c r="C27" s="4"/>
-      <c r="D27" t="s">
-        <v>255</v>
-      </c>
-      <c r="E27" t="s">
-        <v>50</v>
-      </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -1901,6 +1905,12 @@
       <c r="B28" t="s">
         <v>49</v>
       </c>
+      <c r="D28" t="s">
+        <v>257</v>
+      </c>
+      <c r="E28" t="s">
+        <v>50</v>
+      </c>
       <c r="G28" t="s">
         <v>27</v>
       </c>
@@ -1915,12 +1925,6 @@
       <c r="B29" t="s">
         <v>203</v>
       </c>
-      <c r="D29" t="s">
-        <v>256</v>
-      </c>
-      <c r="E29" t="s">
-        <v>50</v>
-      </c>
       <c r="Q29">
         <v>28</v>
       </c>
@@ -1945,12 +1949,6 @@
       </c>
       <c r="B31" t="s">
         <v>204</v>
-      </c>
-      <c r="D31" t="s">
-        <v>257</v>
-      </c>
-      <c r="E31" t="s">
-        <v>50</v>
       </c>
       <c r="Q31">
         <v>30</v>

</xml_diff>

<commit_message>
added mcu to board.
</commit_message>
<xml_diff>
--- a/dwg/crossbar.xlsx
+++ b/dwg/crossbar.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="262">
   <si>
     <t>PB10</t>
   </si>
@@ -464,9 +464,6 @@
     <t>PB14</t>
   </si>
   <si>
-    <t>MOTOR_IN1</t>
-  </si>
-  <si>
     <t>AF9</t>
   </si>
   <si>
@@ -494,9 +491,6 @@
     <t>SWDIO</t>
   </si>
   <si>
-    <t>MOTOR_IN2</t>
-  </si>
-  <si>
     <t>MCO2</t>
   </si>
   <si>
@@ -798,12 +792,30 @@
   </si>
   <si>
     <t>LED_7</t>
+  </si>
+  <si>
+    <t>TIM1_CHN</t>
+  </si>
+  <si>
+    <t>TIM1_CH2N</t>
+  </si>
+  <si>
+    <t>PUSH_1</t>
+  </si>
+  <si>
+    <t>PUSH_2</t>
+  </si>
+  <si>
+    <t>MOTOR_FWD</t>
+  </si>
+  <si>
+    <t>MOTOR_REV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -955,6 +967,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -990,6 +1019,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1168,9 +1214,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J108" sqref="J108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,7 +1249,7 @@
         <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>29</v>
@@ -1218,10 +1264,10 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>47</v>
@@ -1230,7 +1276,7 @@
         <v>126</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>17</v>
@@ -1247,7 +1293,7 @@
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -1271,7 +1317,7 @@
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -1295,7 +1341,7 @@
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -1316,7 +1362,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="Q5">
         <v>4</v>
@@ -1327,7 +1373,7 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -1351,7 +1397,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1377,10 +1423,10 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E8" t="s">
         <v>50</v>
@@ -1422,7 +1468,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1433,14 +1479,14 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Q10" s="2">
         <v>9</v>
@@ -1455,7 +1501,7 @@
         <v>117</v>
       </c>
       <c r="K11" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="Q11">
         <v>10</v>
@@ -1469,7 +1515,7 @@
         <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E12" t="s">
         <v>50</v>
@@ -1478,10 +1524,10 @@
         <v>56</v>
       </c>
       <c r="H12" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="Q12">
         <v>11</v>
@@ -1500,7 +1546,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1508,7 +1554,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" s="2" t="s">
@@ -1524,30 +1570,30 @@
         <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E14" t="s">
         <v>50</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>216</v>
-      </c>
       <c r="I14" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -1565,7 +1611,7 @@
         <v>66</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E15" t="s">
         <v>67</v>
@@ -1630,10 +1676,10 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -1654,7 +1700,7 @@
         <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E18" t="s">
         <v>50</v>
@@ -1663,11 +1709,11 @@
         <v>26</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M18" s="4"/>
       <c r="O18" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="P18" t="s">
         <v>40</v>
@@ -1694,13 +1740,13 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="P19" s="2" t="s">
         <v>120</v>
@@ -1715,10 +1761,10 @@
         <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D20" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E20" t="s">
         <v>50</v>
@@ -1747,7 +1793,7 @@
       </c>
       <c r="C22" s="4"/>
       <c r="D22" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E22" t="s">
         <v>50</v>
@@ -1780,7 +1826,9 @@
       <c r="C23" s="4"/>
       <c r="E23" s="6"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="G23" t="s">
+        <v>257</v>
+      </c>
       <c r="H23" s="4" t="s">
         <v>140</v>
       </c>
@@ -1802,7 +1850,7 @@
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
@@ -1825,7 +1873,7 @@
         <v>37</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C25" s="4"/>
       <c r="F25" s="4"/>
@@ -1849,11 +1897,11 @@
         <v>38</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E26" t="s">
         <v>50</v>
@@ -1906,7 +1954,7 @@
         <v>49</v>
       </c>
       <c r="D28" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E28" t="s">
         <v>50</v>
@@ -1923,7 +1971,10 @@
         <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="G29" t="s">
+        <v>257</v>
       </c>
       <c r="Q29">
         <v>28</v>
@@ -1948,7 +1999,7 @@
         <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="Q31">
         <v>30</v>
@@ -2014,11 +2065,11 @@
         <v>1</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="L35" s="2"/>
       <c r="M35" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -2038,7 +2089,7 @@
         <v>13</v>
       </c>
       <c r="G36" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J36" t="s">
         <v>16</v>
@@ -2067,7 +2118,7 @@
       <c r="I37"/>
       <c r="J37"/>
       <c r="K37" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="L37"/>
       <c r="M37"/>
@@ -2088,12 +2139,14 @@
       </c>
       <c r="C38"/>
       <c r="F38"/>
-      <c r="G38"/>
+      <c r="G38" t="s">
+        <v>256</v>
+      </c>
       <c r="H38"/>
       <c r="I38"/>
       <c r="J38"/>
       <c r="K38" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="L38"/>
       <c r="M38"/>
@@ -2112,11 +2165,14 @@
       <c r="B39" t="s">
         <v>145</v>
       </c>
+      <c r="G39" t="s">
+        <v>257</v>
+      </c>
       <c r="K39" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="O39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="Q39">
         <v>38</v>
@@ -2130,6 +2186,9 @@
       <c r="B40" t="s">
         <v>30</v>
       </c>
+      <c r="G40" t="s">
+        <v>256</v>
+      </c>
       <c r="Q40">
         <v>39</v>
       </c>
@@ -2139,7 +2198,7 @@
         <v>55</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C41" s="4"/>
       <c r="E41" s="4"/>
@@ -2151,7 +2210,7 @@
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
@@ -2192,7 +2251,7 @@
         <v>57</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C43" s="4"/>
       <c r="F43" s="4"/>
@@ -2360,7 +2419,7 @@
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
@@ -2384,7 +2443,7 @@
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
@@ -2426,7 +2485,7 @@
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
       <c r="P51" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="Q51" s="2" t="s">
         <v>131</v>
@@ -2440,7 +2499,7 @@
         <v>71</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -2456,7 +2515,7 @@
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
       <c r="P52" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q52" s="2" t="s">
         <v>131</v>
@@ -2470,7 +2529,7 @@
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
@@ -2494,7 +2553,7 @@
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
@@ -2518,7 +2577,7 @@
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
@@ -2542,7 +2601,7 @@
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
@@ -2566,7 +2625,7 @@
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
@@ -2590,7 +2649,7 @@
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
@@ -2614,7 +2673,7 @@
         <v>12</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -2630,7 +2689,7 @@
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
       <c r="P59" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="Q59" s="2"/>
       <c r="R59" s="2">
@@ -2642,7 +2701,7 @@
         <v>13</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -2658,7 +2717,7 @@
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
       <c r="P60" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="Q60" s="2"/>
       <c r="R60" s="2">
@@ -2698,7 +2757,7 @@
         <v>9</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -2714,7 +2773,7 @@
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
       <c r="P62" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="Q62" s="2"/>
       <c r="R62" s="2">
@@ -2735,7 +2794,7 @@
         <v>50</v>
       </c>
       <c r="I63" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="R63">
         <v>11</v>
@@ -2746,7 +2805,10 @@
         <v>7</v>
       </c>
       <c r="B64" t="s">
-        <v>185</v>
+        <v>183</v>
+      </c>
+      <c r="D64" t="s">
+        <v>259</v>
       </c>
       <c r="R64">
         <v>12</v>
@@ -2774,7 +2836,13 @@
         <v>4</v>
       </c>
       <c r="B66" t="s">
-        <v>201</v>
+        <v>199</v>
+      </c>
+      <c r="D66" t="s">
+        <v>258</v>
+      </c>
+      <c r="E66" t="s">
+        <v>50</v>
       </c>
       <c r="I66" t="s">
         <v>137</v>
@@ -2805,7 +2873,7 @@
         <v>2</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -2821,7 +2889,7 @@
       <c r="N68" s="2"/>
       <c r="O68" s="2"/>
       <c r="P68" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="Q68" s="2"/>
       <c r="R68" s="2">
@@ -2849,7 +2917,7 @@
       <c r="N69" s="2"/>
       <c r="O69" s="2"/>
       <c r="P69" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="Q69" s="2"/>
       <c r="R69" s="2">
@@ -2861,7 +2929,7 @@
         <v>98</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -2877,7 +2945,7 @@
       <c r="N70" s="2"/>
       <c r="O70" s="2"/>
       <c r="P70" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="Q70" s="2"/>
       <c r="R70" s="2">
@@ -2901,13 +2969,13 @@
         <v>92</v>
       </c>
       <c r="I71" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J71" t="s">
         <v>7</v>
       </c>
       <c r="L71" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="R71">
         <v>19</v>
@@ -2929,13 +2997,13 @@
         <v>94</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J72" s="2" t="s">
         <v>15</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="L72" s="2"/>
       <c r="M72" s="2"/>
@@ -2954,7 +3022,7 @@
         <v>94</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
@@ -2977,7 +3045,7 @@
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="R74" s="4">
         <v>22</v>
@@ -3004,7 +3072,7 @@
       </c>
       <c r="K75" s="2"/>
       <c r="L75" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="M75" s="2" t="s">
         <v>48</v>
@@ -3040,10 +3108,10 @@
       </c>
       <c r="K76" s="4"/>
       <c r="L76" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="M76" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="R76">
         <v>24</v>
@@ -3057,13 +3125,13 @@
         <v>61</v>
       </c>
       <c r="F77" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H77" t="s">
         <v>60</v>
       </c>
       <c r="K77" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="R77">
         <v>25</v>
@@ -3074,7 +3142,7 @@
         <v>91</v>
       </c>
       <c r="B78" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C78"/>
       <c r="D78"/>
@@ -3087,7 +3155,7 @@
       <c r="I78"/>
       <c r="J78"/>
       <c r="K78" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="L78"/>
       <c r="M78"/>
@@ -3104,7 +3172,7 @@
         <v>88</v>
       </c>
       <c r="B79" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C79"/>
       <c r="D79"/>
@@ -3130,16 +3198,16 @@
         <v>89</v>
       </c>
       <c r="B80" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F80" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G80" t="s">
         <v>56</v>
       </c>
       <c r="K80" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="R80">
         <v>28</v>
@@ -3180,7 +3248,7 @@
         <v>87</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C82" s="4"/>
       <c r="F82" s="4"/>
@@ -3191,7 +3259,7 @@
       <c r="K82" s="4"/>
       <c r="L82" s="4"/>
       <c r="M82" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="N82" s="4"/>
       <c r="O82" s="4"/>
@@ -3206,7 +3274,7 @@
         <v>84</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C83" s="4"/>
       <c r="E83" s="4"/>
@@ -3231,7 +3299,7 @@
         <v>85</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
@@ -3247,7 +3315,7 @@
       <c r="N84" s="2"/>
       <c r="O84" s="2"/>
       <c r="P84" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="Q84" s="2"/>
       <c r="R84" s="2">
@@ -3259,7 +3327,7 @@
         <v>82</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C85" s="4"/>
       <c r="E85" s="4"/>
@@ -3284,11 +3352,11 @@
         <v>83</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C86" s="4"/>
       <c r="D86" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E86" s="4" t="s">
         <v>50</v>
@@ -3302,7 +3370,7 @@
       <c r="L86" s="4"/>
       <c r="M86" s="4"/>
       <c r="N86" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O86" s="4"/>
       <c r="P86" s="4"/>
@@ -3316,7 +3384,7 @@
         <v>80</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
@@ -3328,13 +3396,13 @@
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
       <c r="L87" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
       <c r="O87" s="2"/>
       <c r="P87" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="Q87" s="2"/>
       <c r="R87" s="2">
@@ -3346,11 +3414,11 @@
         <v>81</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C88" s="4"/>
       <c r="D88" t="s">
-        <v>146</v>
+        <v>260</v>
       </c>
       <c r="E88" t="s">
         <v>50</v>
@@ -3376,7 +3444,7 @@
         <v>78</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
@@ -3388,17 +3456,17 @@
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
       <c r="L89" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="M89" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="N89" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="O89" s="2"/>
       <c r="P89" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="Q89" s="2"/>
       <c r="R89" s="2">
@@ -3410,22 +3478,22 @@
         <v>80</v>
       </c>
       <c r="B90" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D90" t="s">
-        <v>156</v>
+        <v>261</v>
       </c>
       <c r="E90" t="s">
         <v>50</v>
       </c>
       <c r="L90" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="M90" t="s">
         <v>108</v>
       </c>
       <c r="N90" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R90">
         <v>38</v>
@@ -3436,13 +3504,13 @@
         <v>76</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
@@ -3454,7 +3522,7 @@
       <c r="N91" s="2"/>
       <c r="O91" s="2"/>
       <c r="P91" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="Q91" s="2"/>
       <c r="R91" s="2">
@@ -3466,13 +3534,13 @@
         <v>77</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
       <c r="F92" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G92" s="5" t="s">
         <v>54</v>
@@ -3481,10 +3549,10 @@
       <c r="I92" s="5"/>
       <c r="J92" s="5"/>
       <c r="K92" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="L92" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="M92" s="5"/>
       <c r="N92" s="5"/>
@@ -3515,7 +3583,7 @@
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
       <c r="M93" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="N93" s="2"/>
       <c r="O93" s="2"/>
@@ -3532,13 +3600,13 @@
         <v>72</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
       <c r="F94" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
@@ -3550,7 +3618,7 @@
       <c r="N94" s="2"/>
       <c r="O94" s="2"/>
       <c r="P94" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Q94" s="2"/>
       <c r="R94" s="2">
@@ -3619,13 +3687,13 @@
         <v>65</v>
       </c>
       <c r="B97" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H97" t="s">
         <v>140</v>
       </c>
       <c r="I97" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="R97">
         <v>45</v>
@@ -3645,13 +3713,13 @@
         <v>123</v>
       </c>
       <c r="F98" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H98" t="s">
         <v>123</v>
       </c>
       <c r="I98" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J98" t="s">
         <v>14</v>
@@ -3680,7 +3748,7 @@
         <v>125</v>
       </c>
       <c r="N99" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="P99" t="s">
         <v>127</v>
@@ -3694,7 +3762,7 @@
         <v>64</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
@@ -3705,18 +3773,18 @@
         <v>26</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
       <c r="M100" s="2"/>
       <c r="N100" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O100" s="2"/>
       <c r="P100" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="Q100" s="2"/>
       <c r="R100" s="2">
@@ -3728,7 +3796,7 @@
       <c r="B101" s="6"/>
       <c r="C101" s="6"/>
       <c r="D101" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E101" s="6"/>
       <c r="F101" s="6"/>
@@ -3752,7 +3820,7 @@
       <c r="B102" s="6"/>
       <c r="C102" s="6"/>
       <c r="D102" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E102" s="6"/>
       <c r="F102" s="6"/>
@@ -3816,7 +3884,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3859,7 +3927,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B5" t="s">
         <v>57</v>

</xml_diff>